<commit_message>
added py cleanup, working deck layer
</commit_message>
<xml_diff>
--- a/py/data/stadium_and_matches.xlsx
+++ b/py/data/stadium_and_matches.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wc-travel-18\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wc-travel-tracker\py\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0E46EBFF-F8B5-4F14-AE8D-D0306754B510}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F2C4056D-461D-4948-8520-C125627D4DE1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{437AB7E8-5305-4F35-A56A-F570C42485A9}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="185">
   <si>
     <t>Tournament name</t>
   </si>
@@ -175,9 +175,6 @@
     <t>Attendance</t>
   </si>
   <si>
-    <t>Date (CET)</t>
-  </si>
-  <si>
     <t>14/06/2018 17:00</t>
   </si>
   <si>
@@ -571,18 +568,28 @@
     <t>South Korea  </t>
   </si>
   <si>
-    <t>Team 1</t>
-  </si>
-  <si>
-    <t>Team 2</t>
+    <t>PctAttendance</t>
+  </si>
+  <si>
+    <t>DatePlayed</t>
+  </si>
+  <si>
+    <t>Date_Format_CET</t>
+  </si>
+  <si>
+    <t>Team_1</t>
+  </si>
+  <si>
+    <t>Team_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -627,7 +634,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -637,9 +644,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1121,7 +1127,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E8">
         <v>56.337499999999999</v>
@@ -1141,7 +1147,7 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E9">
         <v>55.818837000000002</v>
@@ -1161,7 +1167,7 @@
         <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E10">
         <v>53.277777999999998</v>
@@ -1181,7 +1187,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E11">
         <v>54.182777999999999</v>
@@ -1201,7 +1207,7 @@
         <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E12">
         <v>54.698056000000001</v>
@@ -1221,7 +1227,7 @@
         <v>37</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E13">
         <v>56.832500000000003</v>
@@ -1238,27 +1244,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822AD5D7-4E2C-48B9-B8AB-FC91B1776EB8}">
-  <dimension ref="A1:M92"/>
+  <dimension ref="A1:K92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="26.42578125" style="11" customWidth="1"/>
-    <col min="11" max="11" width="26.42578125" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
         <v>47</v>
@@ -1266,19 +1273,25 @@
       <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="11" t="s">
+      <c r="D1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1289,19 +1302,22 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="H2" s="10">
+        <v>43265.708333333336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
@@ -1312,19 +1328,22 @@
       <c r="D3" s="3">
         <v>0.81699999999999995</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="11" t="s">
+      <c r="E3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H3" s="10">
+        <v>43266.583333333336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1335,22 +1354,25 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="10">
+        <v>43270.833333333336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="1">
         <v>42678</v>
@@ -1358,19 +1380,22 @@
       <c r="D5" s="3">
         <v>0.98199999999999998</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="H5" s="10">
+        <v>43271.708333333336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
@@ -1381,19 +1406,22 @@
       <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="11" t="s">
+      <c r="E6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="I6" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H6" s="10">
+        <v>43276.666666666664</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -1404,20 +1432,22 @@
       <c r="D7" s="3">
         <v>0.84199999999999997</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="J7"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H7" s="10">
+        <v>43276.666666666664</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -1428,19 +1458,22 @@
       <c r="D8" s="2">
         <v>0.97</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="11" t="s">
+      <c r="E8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H8" s="10">
+        <v>43266.708333333336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -1451,19 +1484,22 @@
       <c r="D9" s="2">
         <v>0.99</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="11" t="s">
+      <c r="E9" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="I9" s="11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H9" s="10">
+        <v>43266.833333333336</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -1474,20 +1510,23 @@
       <c r="D10" s="2">
         <v>1</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="K10" s="11"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H10" s="10">
+        <v>43271.583333333336</v>
+      </c>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
@@ -1498,20 +1537,23 @@
       <c r="D11" s="3">
         <v>0.996</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="K11" s="11"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H11" s="10">
+        <v>43271.833333333336</v>
+      </c>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
@@ -1522,20 +1564,23 @@
       <c r="D12" s="2">
         <v>1</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="11" t="s">
+      <c r="E12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="I12" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="K12" s="11"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H12" s="10">
+        <v>43276.833333333336</v>
+      </c>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
@@ -1546,20 +1591,23 @@
       <c r="D13" s="2">
         <v>1</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="K13" s="11"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E13" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H13" s="10">
+        <v>43276.833333333336</v>
+      </c>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
@@ -1570,19 +1618,22 @@
       <c r="D14" s="3">
         <v>0.96299999999999997</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="11" t="s">
+      <c r="E14" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="I14" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H14" s="10">
+        <v>43267.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
@@ -1593,19 +1644,22 @@
       <c r="D15" s="3">
         <v>0.97199999999999998</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="11" t="s">
+      <c r="E15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="I15" s="11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H15" s="10">
+        <v>43267.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
@@ -1616,20 +1670,23 @@
       <c r="D16" s="2">
         <v>0.97</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="K16" s="11"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="H16" s="10">
+        <v>43272.583333333336</v>
+      </c>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
@@ -1640,20 +1697,23 @@
       <c r="D17" s="3">
         <v>0.99199999999999999</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="K17" s="11"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" s="10">
+        <v>43272.708333333336</v>
+      </c>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -1664,20 +1724,23 @@
       <c r="D18" s="2">
         <v>1</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="K18" s="11"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E18" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="H18" s="10">
+        <v>43277.666666666664</v>
+      </c>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
@@ -1688,20 +1751,23 @@
       <c r="D19" s="3">
         <v>0.995</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="K19" s="11"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E19" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="H19" s="10">
+        <v>43277.666666666664</v>
+      </c>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
@@ -1712,19 +1778,22 @@
       <c r="D20" s="2">
         <v>1</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G20" s="11" t="s">
+      <c r="E20" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="I20" s="11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H20" s="10">
+        <v>43267.625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
         <v>32</v>
@@ -1735,19 +1804,22 @@
       <c r="D21" s="3">
         <v>0.91600000000000004</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G21" s="11" t="s">
+      <c r="E21" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="I21" s="11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H21" s="10">
+        <v>43267.875</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
@@ -1758,20 +1830,23 @@
       <c r="D22" s="2">
         <v>1</v>
       </c>
-      <c r="F22" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="K22" s="11"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E22" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="H22" s="10">
+        <v>43272.833333333336</v>
+      </c>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
@@ -1782,20 +1857,23 @@
       <c r="D23" s="3">
         <v>0.93600000000000005</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="K23" s="11"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E23" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="H23" s="10">
+        <v>43273.708333333336</v>
+      </c>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -1806,23 +1884,26 @@
       <c r="D24" s="2">
         <v>1</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" s="11" t="s">
+      <c r="E24" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="I24" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="K24" s="11"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H24" s="10">
+        <v>43277.833333333336</v>
+      </c>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C25" s="1">
         <v>43472</v>
@@ -1830,20 +1911,23 @@
       <c r="D25" s="2">
         <v>1</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="K25" s="11"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E25" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="H25" s="10">
+        <v>43277.833333333336</v>
+      </c>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
@@ -1854,23 +1938,25 @@
       <c r="D26" s="7">
         <v>0.98699999999999999</v>
       </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E26" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="H26" s="10">
+        <v>43268.583333333336</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C27" s="1">
         <v>43109</v>
@@ -1878,22 +1964,23 @@
       <c r="D27" s="7">
         <v>0.99199999999999999</v>
       </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" s="11" t="s">
+      <c r="E27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G27" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="H27" s="10"/>
-      <c r="I27" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="K27" s="11"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H27" s="10">
+        <v>43268.833333333336</v>
+      </c>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -1904,22 +1991,23 @@
       <c r="D28" s="7">
         <v>1</v>
       </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="H28" s="9"/>
-      <c r="I28" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="K28" s="11"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E28" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H28" s="10">
+        <v>43273.583333333336</v>
+      </c>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
@@ -1930,22 +2018,23 @@
       <c r="D29" s="7">
         <v>0.97599999999999998</v>
       </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="H29" s="10"/>
-      <c r="I29" s="11" t="s">
+      <c r="E29" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="K29" s="11"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G29" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H29" s="10">
+        <v>43273.833333333336</v>
+      </c>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
@@ -1956,20 +2045,23 @@
       <c r="D30" s="7">
         <v>1</v>
       </c>
-      <c r="F30" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G30" s="11" t="s">
+      <c r="E30" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G30" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="I30" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="K30" s="11"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H30" s="10">
+        <v>43278.833333333336</v>
+      </c>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
         <v>20</v>
@@ -1980,21 +2072,23 @@
       <c r="D31" s="7">
         <v>1</v>
       </c>
-      <c r="F31" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H31" s="10"/>
-      <c r="I31" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="K31" s="11"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E31" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H31" s="10">
+        <v>43278.833333333336</v>
+      </c>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
@@ -2005,20 +2099,23 @@
       <c r="D32" s="7">
         <v>1</v>
       </c>
-      <c r="F32" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G32" s="11" t="s">
+      <c r="E32" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G32" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="I32" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="K32" s="11"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H32" s="10">
+        <v>43268.708333333336</v>
+      </c>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B33" t="s">
         <v>20</v>
@@ -2029,24 +2126,26 @@
       <c r="D33" s="7">
         <v>0.97599999999999998</v>
       </c>
-      <c r="F33" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="H33" s="9"/>
-      <c r="I33" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="K33" s="11"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E33" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="H33" s="10">
+        <v>43269.583333333336</v>
+      </c>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C34" s="1">
         <v>43472</v>
@@ -2054,20 +2153,22 @@
       <c r="D34" s="7">
         <v>1</v>
       </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E34" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H34" s="10">
+        <v>43274.708333333336</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B35" t="s">
         <v>9</v>
@@ -2078,21 +2179,22 @@
       <c r="D35" s="7">
         <v>1</v>
       </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="H35" s="10"/>
-      <c r="I35" s="11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E35" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H35" s="10">
+        <v>43274.833333333336</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
         <v>23</v>
@@ -2103,20 +2205,22 @@
       <c r="D36" s="7">
         <v>0.97599999999999998</v>
       </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="I36" s="11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E36" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="H36" s="10">
+        <v>43278.666666666664</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
@@ -2127,21 +2231,23 @@
       <c r="D37" s="7">
         <v>1</v>
       </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="I37" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="K37" s="11"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E37" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H37" s="10">
+        <v>43278.666666666664</v>
+      </c>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
         <v>9</v>
@@ -2152,22 +2258,23 @@
       <c r="D38" s="7">
         <v>0.97699999999999998</v>
       </c>
-      <c r="E38" s="1"/>
-      <c r="F38" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G38" s="11" t="s">
+      <c r="E38" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G38" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H38" s="9"/>
-      <c r="I38" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="K38" s="11"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H38" s="10">
+        <v>43269.708333333336</v>
+      </c>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" t="s">
         <v>14</v>
@@ -2178,22 +2285,23 @@
       <c r="D39" s="7">
         <v>0.93899999999999995</v>
       </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G39" s="11" t="s">
+      <c r="E39" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G39" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H39" s="10"/>
-      <c r="I39" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="K39" s="11"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H39" s="10">
+        <v>43269.833333333336</v>
+      </c>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B40" t="s">
         <v>12</v>
@@ -2204,24 +2312,26 @@
       <c r="D40" s="7">
         <v>1</v>
       </c>
-      <c r="F40" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="H40" s="10"/>
-      <c r="I40" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="K40" s="11"/>
-      <c r="M40" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E40" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H40" s="10">
+        <v>43274.583333333336</v>
+      </c>
+      <c r="I40" s="9"/>
+      <c r="K40" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B41" t="s">
         <v>20</v>
@@ -2232,21 +2342,23 @@
       <c r="D41" s="7">
         <v>1</v>
       </c>
-      <c r="F41" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="H41" s="10"/>
-      <c r="I41" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="K41" s="11"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E41" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H41" s="10">
+        <v>43275.583333333336</v>
+      </c>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B42" t="s">
         <v>32</v>
@@ -2257,20 +2369,23 @@
       <c r="D42" s="7">
         <v>1</v>
       </c>
-      <c r="F42" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G42" s="11" t="s">
+      <c r="E42" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G42" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="I42" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="K42" s="11"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H42" s="10">
+        <v>43279.833333333336</v>
+      </c>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B43" t="s">
         <v>29</v>
@@ -2281,21 +2396,23 @@
       <c r="D43" s="7">
         <v>0.89200000000000002</v>
       </c>
-      <c r="F43" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G43" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="H43" s="10"/>
-      <c r="I43" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="K43" s="11"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E43" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H43" s="10">
+        <v>43279.791666666664</v>
+      </c>
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B44" t="s">
         <v>29</v>
@@ -2306,21 +2423,23 @@
       <c r="D44" s="7">
         <v>0.98</v>
       </c>
-      <c r="F44" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G44" s="11" t="s">
+      <c r="E44" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="G44" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="H44" s="10"/>
-      <c r="I44" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="K44" s="11"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H44" s="10">
+        <v>43270.583333333336</v>
+      </c>
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B45" t="s">
         <v>12</v>
@@ -2331,19 +2450,22 @@
       <c r="D45" s="7">
         <v>1</v>
       </c>
-      <c r="F45" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G45" s="11" t="s">
+      <c r="E45" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="G45" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="I45" s="11" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H45" s="10">
+        <v>43270.708333333336</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B46" t="s">
         <v>35</v>
@@ -2354,21 +2476,23 @@
       <c r="D46" s="7">
         <v>0.98499999999999999</v>
       </c>
-      <c r="F46" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="H46" s="10"/>
-      <c r="I46" s="11" t="s">
+      <c r="E46" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F46" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="K46" s="11"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G46" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H46" s="10">
+        <v>43275.708333333336</v>
+      </c>
+      <c r="I46" s="9"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B47" t="s">
         <v>23</v>
@@ -2379,20 +2503,23 @@
       <c r="D47" s="7">
         <v>1</v>
       </c>
-      <c r="F47" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G47" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="I47" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="K47" s="11"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E47" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="H47" s="10">
+        <v>43275.833333333336</v>
+      </c>
+      <c r="I47" s="9"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B48" t="s">
         <v>14</v>
@@ -2403,20 +2530,23 @@
       <c r="D48" s="7">
         <v>0.96499999999999997</v>
       </c>
-      <c r="F48" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="I48" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="K48" s="11"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E48" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="H48" s="10">
+        <v>43279.666666666664</v>
+      </c>
+      <c r="I48" s="9"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s">
         <v>26</v>
@@ -2427,18 +2557,21 @@
       <c r="D49" s="7">
         <v>1</v>
       </c>
-      <c r="F49" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G49" s="11" t="s">
+      <c r="E49" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G49" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="I49" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="K49" s="11"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H49" s="10">
+        <v>43279.666666666664</v>
+      </c>
+      <c r="I49" s="9"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>16</v>
       </c>
@@ -2451,20 +2584,21 @@
       <c r="D50" s="7">
         <v>1</v>
       </c>
-      <c r="E50" s="5"/>
-      <c r="F50" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="H50" s="10"/>
-      <c r="I50" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="K50" s="11"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E50" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="H50" s="10">
+        <v>43281.666666666664</v>
+      </c>
+      <c r="I50" s="9"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>16</v>
       </c>
@@ -2477,20 +2611,21 @@
       <c r="D51" s="7">
         <v>1</v>
       </c>
-      <c r="E51" s="5"/>
-      <c r="F51" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G51" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="H51" s="10"/>
-      <c r="I51" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="K51" s="11"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E51" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="H51" s="10">
+        <v>43281.833333333336</v>
+      </c>
+      <c r="I51" s="9"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>16</v>
       </c>
@@ -2503,20 +2638,21 @@
       <c r="D52" s="7">
         <v>1</v>
       </c>
-      <c r="E52" s="5"/>
-      <c r="F52" s="8">
+      <c r="E52" s="8">
         <v>43107.666666666664</v>
       </c>
-      <c r="G52" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="H52" s="10"/>
-      <c r="I52" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="L52" s="5"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F52" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="H52" s="10">
+        <v>43282.666666666664</v>
+      </c>
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>16</v>
       </c>
@@ -2529,20 +2665,21 @@
       <c r="D53" s="7">
         <v>0.94299999999999995</v>
       </c>
-      <c r="E53" s="5"/>
-      <c r="F53" s="8">
+      <c r="E53" s="8">
         <v>43107.833333333336</v>
       </c>
-      <c r="G53" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="H53" s="10"/>
-      <c r="I53" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="L53" s="5"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F53" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="H53" s="10">
+        <v>43282.833333333336</v>
+      </c>
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>16</v>
       </c>
@@ -2555,26 +2692,27 @@
       <c r="D54" s="7">
         <v>1</v>
       </c>
-      <c r="E54" s="5"/>
-      <c r="F54" s="8">
+      <c r="E54" s="8">
         <v>43138.666666666664</v>
       </c>
-      <c r="G54" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="H54" s="9"/>
-      <c r="I54" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="K54" s="11"/>
-      <c r="M54" s="5"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F54" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H54" s="10">
+        <v>43283.666666666664</v>
+      </c>
+      <c r="I54" s="9"/>
+      <c r="K54" s="5"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C55" s="6">
         <v>41466</v>
@@ -2582,21 +2720,22 @@
       <c r="D55" s="7">
         <v>0.95399999999999996</v>
       </c>
-      <c r="E55" s="5"/>
-      <c r="F55" s="8">
+      <c r="E55" s="8">
         <v>43138.833333333336</v>
       </c>
-      <c r="G55" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="H55" s="10"/>
-      <c r="I55" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="K55" s="11"/>
-      <c r="M55" s="5"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F55" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="H55" s="10">
+        <v>43283.833333333336</v>
+      </c>
+      <c r="I55" s="9"/>
+      <c r="K55" s="5"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>16</v>
       </c>
@@ -2609,20 +2748,22 @@
       <c r="D56" s="7">
         <v>0.99299999999999999</v>
       </c>
-      <c r="F56" s="8">
+      <c r="E56" s="8">
         <v>43166.666666666664</v>
       </c>
-      <c r="G56" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="H56" s="9"/>
-      <c r="I56" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="K56" s="11"/>
-      <c r="M56" s="5"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F56" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H56" s="10">
+        <v>43284.666666666664</v>
+      </c>
+      <c r="I56" s="9"/>
+      <c r="K56" s="5"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>16</v>
       </c>
@@ -2635,21 +2776,23 @@
       <c r="D57" s="7">
         <v>1</v>
       </c>
-      <c r="F57" s="8">
+      <c r="E57" s="8">
         <v>43166.833333333336</v>
       </c>
-      <c r="G57" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="H57" s="10"/>
-      <c r="I57" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="L57" s="5"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F57" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H57" s="10">
+        <v>43284.833333333336</v>
+      </c>
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B58" t="s">
         <v>20</v>
@@ -2660,21 +2803,24 @@
       <c r="D58" s="2">
         <v>1</v>
       </c>
-      <c r="F58" s="8">
+      <c r="E58" s="8">
         <v>43258.666666666664</v>
       </c>
-      <c r="G58" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="I58" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="K58" s="11"/>
-      <c r="M58" s="5"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F58" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="H58" s="10">
+        <v>43287.666666666664</v>
+      </c>
+      <c r="I58" s="9"/>
+      <c r="K58" s="5"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B59" t="s">
         <v>23</v>
@@ -2685,22 +2831,24 @@
       <c r="D59" s="2">
         <v>1</v>
       </c>
-      <c r="F59" s="8">
+      <c r="E59" s="8">
         <v>43258.833333333336</v>
       </c>
-      <c r="G59" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="H59" s="10"/>
-      <c r="I59" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="K59" s="11"/>
-      <c r="M59" s="5"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F59" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="H59" s="10">
+        <v>43287.833333333336</v>
+      </c>
+      <c r="I59" s="9"/>
+      <c r="K59" s="5"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B60" t="s">
         <v>26</v>
@@ -2711,21 +2859,24 @@
       <c r="D60" s="3">
         <v>0.95299999999999996</v>
       </c>
-      <c r="F60" s="8">
+      <c r="E60" s="8">
         <v>43288.666666666664</v>
       </c>
-      <c r="G60" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="I60" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="K60" s="11"/>
-      <c r="M60" s="5"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F60" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H60" s="10">
+        <v>43288.666666666664</v>
+      </c>
+      <c r="I60" s="9"/>
+      <c r="K60" s="5"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
@@ -2736,21 +2887,23 @@
       <c r="D61" s="2">
         <v>1</v>
       </c>
-      <c r="F61" s="8">
+      <c r="E61" s="8">
         <v>43288.833333333336</v>
       </c>
-      <c r="G61" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H61" s="10"/>
-      <c r="I61" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="L61" s="5"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F61" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="H61" s="10">
+        <v>43288.833333333336</v>
+      </c>
+      <c r="J61" s="5"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
         <v>6</v>
@@ -2761,22 +2914,24 @@
       <c r="D62" s="3">
         <v>0.997</v>
       </c>
-      <c r="F62" s="8">
+      <c r="E62" s="8">
         <v>43380.833333333336</v>
       </c>
-      <c r="G62" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="H62" s="9"/>
-      <c r="I62" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="K62" s="11"/>
-      <c r="M62" s="5"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F62" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="H62" s="10">
+        <v>43291.833333333336</v>
+      </c>
+      <c r="I62" s="9"/>
+      <c r="K62" s="5"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B63" t="s">
         <v>3</v>
@@ -2787,135 +2942,143 @@
       <c r="D63" s="2">
         <v>1</v>
       </c>
-      <c r="F63" s="8">
+      <c r="E63" s="8">
         <v>43411.833333333336</v>
       </c>
-      <c r="G63" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="H63" s="10"/>
-      <c r="I63" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="K63" s="11"/>
-      <c r="M63" s="5"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F63" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H63" s="10">
+        <v>43292.833333333336</v>
+      </c>
+      <c r="I63" s="9"/>
+      <c r="K63" s="5"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B64" t="s">
         <v>6</v>
       </c>
-      <c r="F64" t="s">
-        <v>110</v>
-      </c>
-      <c r="G64" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="I64" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="K64" s="11"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>109</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H64" s="10">
+        <v>43295.666666666664</v>
+      </c>
+      <c r="I64" s="9"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B65" t="s">
         <v>3</v>
       </c>
-      <c r="F65" t="s">
-        <v>111</v>
-      </c>
-      <c r="G65" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="I65" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="K65" s="11"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F66"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F67"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F68"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F69"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F70"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F71"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F72"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F73"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F74"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F75"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F76"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F77"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F78"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F79"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F80"/>
-    </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F81"/>
-    </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F82"/>
-    </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F83"/>
-    </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F84"/>
-    </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F85"/>
-    </row>
-    <row r="86" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F86"/>
-    </row>
-    <row r="87" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F87"/>
-    </row>
-    <row r="88" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F88"/>
-    </row>
-    <row r="89" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F89"/>
-    </row>
-    <row r="90" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F90"/>
-    </row>
-    <row r="91" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F91"/>
-    </row>
-    <row r="92" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F92"/>
+      <c r="E65" t="s">
+        <v>110</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="H65" s="10">
+        <v>43296.708333333336</v>
+      </c>
+      <c r="I65" s="9"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E66"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E67"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E68"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E69"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E70"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E71"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E72"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E73"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E74"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E75"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E76"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E77"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E78"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E79"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E80"/>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E81"/>
+    </row>
+    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E82"/>
+    </row>
+    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E83"/>
+    </row>
+    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E84"/>
+    </row>
+    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E85"/>
+    </row>
+    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E86"/>
+    </row>
+    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E87"/>
+    </row>
+    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E88"/>
+    </row>
+    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E89"/>
+    </row>
+    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E90"/>
+    </row>
+    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E91"/>
+    </row>
+    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E92"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>